<commit_message>
Added death counts from 27/04-2021
</commit_message>
<xml_diff>
--- a/DanskeData/DeathsAgeDK/Deaths.xlsx
+++ b/DanskeData/DeathsAgeDK/Deaths.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rucdk-my.sharepoint.com/personal/rakrpe_ruc_dk/Documents/Pandemix/SSI/DeathsAgeDK/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rakrpe\Documents\PandemiX\GithubRepos\PandemiX\DanskeData\DeathsAgeDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>0-9</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Aldersgruppe</t>
+  </si>
+  <si>
+    <t>27_04_2021</t>
   </si>
 </sst>
 </file>
@@ -450,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -534,8 +537,11 @@
       <c r="Y1" t="s">
         <v>34</v>
       </c>
+      <c r="Z1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,8 +617,11 @@
       <c r="Y2">
         <v>1</v>
       </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -688,8 +697,11 @@
       <c r="Y3">
         <v>0</v>
       </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -765,8 +777,11 @@
       <c r="Y4">
         <v>0</v>
       </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -842,8 +857,11 @@
       <c r="Y5">
         <v>6</v>
       </c>
+      <c r="Z5">
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -919,8 +937,11 @@
       <c r="Y6">
         <v>7</v>
       </c>
+      <c r="Z6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -996,8 +1017,11 @@
       <c r="Y7">
         <v>59</v>
       </c>
+      <c r="Z7">
+        <v>60</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1073,8 +1097,11 @@
       <c r="Y8">
         <v>205</v>
       </c>
+      <c r="Z8">
+        <v>207</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1150,8 +1177,11 @@
       <c r="Y9">
         <v>647</v>
       </c>
+      <c r="Z9">
+        <v>651</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1227,8 +1257,11 @@
       <c r="Y10">
         <v>984</v>
       </c>
+      <c r="Z10">
+        <v>988</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1304,8 +1337,11 @@
       <c r="Y11">
         <v>554</v>
       </c>
+      <c r="Z11">
+        <v>557</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1398,12 +1434,16 @@
         <v>2432</v>
       </c>
       <c r="X12">
-        <f t="shared" ref="X12:Y12" si="13">SUM(X2:X11)</f>
+        <f t="shared" ref="X12:Z12" si="13">SUM(X2:X11)</f>
         <v>2446</v>
       </c>
       <c r="Y12">
         <f t="shared" si="13"/>
         <v>2463</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="13"/>
+        <v>2479</v>
       </c>
     </row>
   </sheetData>
@@ -1413,6 +1453,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010067B0F61001E26E4990655038295DAB15" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ee3cdd56ad75a133cec0310dc1ffbdf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c985db34-e54d-4323-9c17-343881a3f777" xmlns:ns4="43c47581-a1ab-43e4-9644-f9cb95e620d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dce359d01537b7c93672f0fb6f914998" ns3:_="" ns4:_="">
     <xsd:import namespace="c985db34-e54d-4323-9c17-343881a3f777"/>
@@ -1615,15 +1664,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1631,6 +1671,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B0378E4-CD70-4312-8DC0-09A17EAA3240}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1645,14 +1693,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAEE481-A366-4836-8CFB-49F219EE660D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>